<commit_message>
Recalibrates, updates code for plots
</commit_message>
<xml_diff>
--- a/data/2023_fuel_usage.xlsx
+++ b/data/2023_fuel_usage.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettdevine/repos/h2-adoption-model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEC85654-BAE7-9141-8C6F-7449D113E9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00775417-AF70-2E41-9186-1D68B0D4B6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="2220" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="15020" yWindow="8480" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023_fuel_usage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1" iterateDelta="1.0000000000000001E-5" calcOnSave="0"/>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -907,11 +908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,6 +920,7 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>